<commit_message>
se agrego el documentos con los esquemas de la metodologia
</commit_message>
<xml_diff>
--- a/docs/metrics.xlsx
+++ b/docs/metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS TUF\Documents\repositorios\energy_consumption\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525C30C5-1A40-404F-94F6-56418D31A33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7125FC7-6493-4C3D-9EEB-55025DF7F9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -483,13 +483,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -812,19 +812,19 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>124</v>
       </c>
     </row>
@@ -835,13 +835,13 @@
       <c r="E5" t="s">
         <v>126</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>3</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>0.82899999999999996</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>0.3</v>
       </c>
     </row>
@@ -852,13 +852,13 @@
       <c r="E6" t="s">
         <v>127</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>14</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>0.59399999999999997</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>0.98899999999999999</v>
       </c>
     </row>
@@ -869,13 +869,13 @@
       <c r="E7" t="s">
         <v>128</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>4</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>0.84099999999999997</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>0.14399999999999999</v>
       </c>
     </row>
@@ -886,13 +886,13 @@
       <c r="E8" t="s">
         <v>126</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>3</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>0.78300000000000003</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>0.49299999999999999</v>
       </c>
     </row>
@@ -903,13 +903,13 @@
       <c r="E9" t="s">
         <v>127</v>
       </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -920,13 +920,13 @@
       <c r="E10" t="s">
         <v>128</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>4</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>0.81299999999999994</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>0.17899999999999999</v>
       </c>
     </row>
@@ -940,7 +940,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="O1" sqref="O1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -958,34 +958,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="L1" s="4"/>
+      <c r="M1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
+      <c r="N1" s="4"/>
+      <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1044,46 +1044,46 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1094,46 +1094,46 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1144,46 +1144,46 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1194,46 +1194,46 @@
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>3.1438429999999998E-13</v>
       </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
         <v>1.0178E-2</v>
       </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
         <v>5.6231000000000003E-2</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>0.99999400000000005</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>1.208405</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>0.99717199999999995</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="2">
         <v>3.1438429999999998E-13</v>
       </c>
-      <c r="L6" s="3">
-        <v>1</v>
-      </c>
-      <c r="M6" s="3">
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
         <v>3.1512999999999999E-2</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="2">
         <v>0.99999800000000005</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="2">
         <v>4.5643999999999997E-2</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="2">
         <v>0.999996</v>
       </c>
     </row>
@@ -1244,46 +1244,46 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P7" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1294,46 +1294,46 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1344,46 +1344,46 @@
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M9" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="O9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="P9" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1394,46 +1394,46 @@
       <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>1.331954E-13</v>
       </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
         <v>1.0085999999999999E-2</v>
       </c>
-      <c r="F10" s="3">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
         <v>0.46712100000000001</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>0.99999899999999997</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>54.683965999999998</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>0.98627699999999996</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="2">
         <v>1.331954E-13</v>
       </c>
-      <c r="L10" s="3">
-        <v>1</v>
-      </c>
-      <c r="M10" s="3">
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2">
         <v>0.26831899999999997</v>
       </c>
-      <c r="N10" s="3">
-        <v>1</v>
-      </c>
-      <c r="O10" s="3">
+      <c r="N10" s="2">
+        <v>1</v>
+      </c>
+      <c r="O10" s="2">
         <v>0.42979200000000001</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10" s="2">
         <v>0.99999899999999997</v>
       </c>
     </row>
@@ -1444,46 +1444,46 @@
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="M11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="N11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="O11" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="P11" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1494,46 +1494,46 @@
       <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="M12" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="N12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="O12" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="P12" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1544,46 +1544,46 @@
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="M13" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="N13" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="O13" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="P13" s="2" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1594,46 +1594,46 @@
       <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>3.7147349999999998E-13</v>
       </c>
-      <c r="D14" s="3">
-        <v>1</v>
-      </c>
-      <c r="E14" s="3">
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
         <v>1.0175E-2</v>
       </c>
-      <c r="F14" s="3">
-        <v>1</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
         <v>0.318687</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>0.99999800000000005</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <v>83.623318999999995</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <v>0.88862799999999997</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="2">
         <v>3.7147349999999998E-13</v>
       </c>
-      <c r="L14" s="3">
-        <v>1</v>
-      </c>
-      <c r="M14" s="3">
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2">
         <v>0.14743600000000001</v>
       </c>
-      <c r="N14" s="3">
-        <v>1</v>
-      </c>
-      <c r="O14" s="3">
+      <c r="N14" s="2">
+        <v>1</v>
+      </c>
+      <c r="O14" s="2">
         <v>0.19586100000000001</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14" s="2">
         <v>0.99999899999999997</v>
       </c>
     </row>
@@ -1644,46 +1644,46 @@
       <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M15" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="N15" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="O15" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="P15" s="2" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1694,46 +1694,46 @@
       <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="K16" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M16" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="N16" s="3" t="s">
+      <c r="N16" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="O16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="P16" s="2" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1744,46 +1744,46 @@
       <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="M17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="N17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="O17" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="P17" s="3" t="s">
+      <c r="P17" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1794,46 +1794,46 @@
       <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>3.1863629999999998E-13</v>
       </c>
-      <c r="D18" s="3">
-        <v>1</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
         <v>1.001E-2</v>
       </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3">
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
         <v>0.53312999999999999</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <v>0.99999700000000002</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="2">
         <v>74.224798000000007</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="2">
         <v>0.94884599999999997</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18" s="2">
         <v>3.1863629999999998E-13</v>
       </c>
-      <c r="L18" s="3">
-        <v>1</v>
-      </c>
-      <c r="M18" s="3">
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2">
         <v>0.27301500000000001</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18" s="2">
         <v>0.99999899999999997</v>
       </c>
-      <c r="O18" s="3">
+      <c r="O18" s="2">
         <v>0.34965400000000002</v>
       </c>
-      <c r="P18" s="3">
+      <c r="P18" s="2">
         <v>0.99999899999999997</v>
       </c>
     </row>
@@ -1952,34 +1952,34 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="L1" s="4"/>
+      <c r="M1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
+      <c r="N1" s="4"/>
+      <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
se establecio los mejores modelos de regresion para los dos casos de analisis , usando la serie de tiempo mas cercana a cada centroide de cada cluster y usando la serie de tiempo promedio de cada cluster.
</commit_message>
<xml_diff>
--- a/docs/metrics.xlsx
+++ b/docs/metrics.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS TUF\Documents\repositorios\energy_consumption\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7125FC7-6493-4C3D-9EEB-55025DF7F9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5358AC-E1C7-4934-8D47-8EC82E32B44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="clusteringresults" sheetId="3" r:id="rId1"/>
+    <sheet name="clustering_results" sheetId="3" r:id="rId1"/>
     <sheet name="closest_metrics" sheetId="1" r:id="rId2"/>
     <sheet name="average_metrics" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="135">
   <si>
     <t>Cluster</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Model</t>
   </si>
   <si>
-    <t>MEJOR MODELO</t>
-  </si>
-  <si>
     <t>All Features</t>
   </si>
   <si>
@@ -415,6 +412,21 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>MEJORES MODELOS</t>
+  </si>
+  <si>
+    <t>0.998817</t>
+  </si>
+  <si>
+    <t>0.995178</t>
+  </si>
+  <si>
+    <t>0.997862</t>
+  </si>
+  <si>
+    <t>0.997856</t>
   </si>
 </sst>
 </file>
@@ -478,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -491,6 +503,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -798,7 +825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC80A688-2068-44CC-8E31-E1BA3B0A16A2}">
   <dimension ref="D4:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -813,27 +840,27 @@
   <sheetData>
     <row r="4" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D4" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" t="s">
         <v>125</v>
-      </c>
-      <c r="E5" t="s">
-        <v>126</v>
       </c>
       <c r="F5" s="2">
         <v>3</v>
@@ -847,10 +874,10 @@
     </row>
     <row r="6" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F6" s="2">
         <v>14</v>
@@ -864,10 +891,10 @@
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F7" s="2">
         <v>4</v>
@@ -881,10 +908,10 @@
     </row>
     <row r="8" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8" s="2">
         <v>3</v>
@@ -898,27 +925,27 @@
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E9" t="s">
-        <v>127</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F10" s="2">
         <v>4</v>
@@ -937,10 +964,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:P1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1045,46 +1072,46 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="P3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -1095,46 +1122,46 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="H4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -1145,46 +1172,46 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="P5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -1192,7 +1219,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
         <v>3.1438429999999998E-13</v>
@@ -1245,46 +1272,46 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -1295,46 +1322,46 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="P8" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -1345,46 +1372,46 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="P9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -1392,7 +1419,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2">
         <v>1.331954E-13</v>
@@ -1445,46 +1472,46 @@
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="H11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="M11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="M11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="N11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="P11" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -1495,46 +1522,46 @@
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O12" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="N12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="P12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -1545,46 +1572,46 @@
         <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="H13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="M13" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -1592,7 +1619,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2">
         <v>3.7147349999999998E-13</v>
@@ -1645,46 +1672,46 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M15" s="2" t="s">
+      <c r="N15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O15" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="N15" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="P15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -1695,46 +1722,46 @@
         <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M16" s="2" t="s">
+      <c r="N16" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="P16" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
@@ -1745,46 +1772,46 @@
         <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I17" s="2" t="s">
+      <c r="J17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M17" s="2" t="s">
+      <c r="N17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="N17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="P17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -1792,7 +1819,7 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2">
         <v>3.1863629999999998E-13</v>
@@ -1837,98 +1864,101 @@
         <v>0.99999899999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F21" s="1" t="s">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J22" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I23" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1" t="s">
+      <c r="J23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="L23" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="M23" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F22" t="s">
+    <row r="24" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G22" t="s">
+      <c r="J24" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H22" t="s">
+      <c r="K24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I22">
-        <v>0.96962599999999999</v>
-      </c>
-      <c r="J22">
-        <v>0.99817900000000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F23" t="s">
+      <c r="L24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I25" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G23" t="s">
+      <c r="J25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H23" t="s">
+      <c r="K25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I23">
-        <v>31.258579000000001</v>
-      </c>
-      <c r="J23">
-        <v>0.99551599999999996</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F24" t="s">
+      <c r="L25" s="9">
+        <v>31259</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G24" t="s">
+      <c r="J26" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H24" t="s">
+      <c r="K26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I24">
-        <v>15.551539999999999</v>
-      </c>
-      <c r="J24">
-        <v>0.99614800000000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F25" t="s">
+      <c r="L26" s="9">
+        <v>15552</v>
+      </c>
+      <c r="M26" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G25" t="s">
+      <c r="J27" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H25" t="s">
+      <c r="K27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I25">
-        <v>8.9048800000000004</v>
-      </c>
-      <c r="J25">
-        <v>0.99926400000000004</v>
+      <c r="L27" s="9">
+        <v>8905</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="J22:L22"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
@@ -1945,11 +1975,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60578EB-98D6-4F88-B60F-5DF5FAA0FC36}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23:M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C1" s="4" t="s">
@@ -2186,7 +2220,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>3.6130249999999999E-14</v>
@@ -2386,7 +2420,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>8.8240699999999996E-13</v>
@@ -2586,7 +2620,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>4.3866690000000002E-13</v>
@@ -2786,7 +2820,7 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>6.9544349999999999E-14</v>
@@ -2831,98 +2865,101 @@
         <v>0.99999899999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I22" t="s">
-        <v>19</v>
-      </c>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J23" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K24" s="1" t="s">
+      <c r="J24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="L24" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="M24" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I25" t="s">
+    <row r="25" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I25" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L25">
-        <v>1.4931399999999999</v>
-      </c>
-      <c r="M25">
-        <v>0.99881699999999995</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I26" t="s">
+      <c r="L25" s="9">
+        <v>1493</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L26">
-        <v>31.161010000000001</v>
-      </c>
-      <c r="M26">
-        <v>0.99517800000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I27" t="s">
+      <c r="L26" s="9">
+        <v>31161</v>
+      </c>
+      <c r="M26" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J27" t="s">
-        <v>8</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="J27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L27">
-        <v>10.967959</v>
-      </c>
-      <c r="M27">
-        <v>0.99786200000000003</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I28" t="s">
+      <c r="L27" s="9">
+        <v>10968</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J28" t="s">
-        <v>8</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="J28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L28">
-        <v>1.51938</v>
-      </c>
-      <c r="M28">
-        <v>0.99785599999999997</v>
+      <c r="L28" s="9">
+        <v>1519</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="J23:L23"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>

</xml_diff>

<commit_message>
se realizaron las pruebas con los modelos de regresion seleccionados
</commit_message>
<xml_diff>
--- a/docs/metrics.xlsx
+++ b/docs/metrics.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS TUF\Documents\repositorios\energy_consumption\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5358AC-E1C7-4934-8D47-8EC82E32B44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7106E1EC-0E0E-49F1-926F-0853FD0489FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clustering_results" sheetId="3" r:id="rId1"/>
-    <sheet name="closest_metrics" sheetId="1" r:id="rId2"/>
-    <sheet name="average_metrics" sheetId="2" r:id="rId3"/>
+    <sheet name="average_metrics" sheetId="2" r:id="rId2"/>
+    <sheet name="closest_metrics" sheetId="1" r:id="rId3"/>
+    <sheet name="pruebas_regresion" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="133">
   <si>
     <t>Cluster</t>
   </si>
@@ -417,13 +418,7 @@
     <t>MEJORES MODELOS</t>
   </si>
   <si>
-    <t>0.998817</t>
-  </si>
-  <si>
     <t>0.995178</t>
-  </si>
-  <si>
-    <t>0.997862</t>
   </si>
   <si>
     <t>0.997856</t>
@@ -490,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -501,14 +496,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -519,6 +508,13 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,7 +821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC80A688-2068-44CC-8E31-E1BA3B0A16A2}">
   <dimension ref="D4:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -963,11 +959,1012 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60578EB-98D6-4F88-B60F-5DF5FAA0FC36}">
+  <dimension ref="A1:P28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="9"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>3.5910000000000002</v>
+      </c>
+      <c r="D3">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="E3">
+        <v>3.5910000000000002</v>
+      </c>
+      <c r="F3">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="G3">
+        <v>1.349</v>
+      </c>
+      <c r="H3">
+        <v>0.998</v>
+      </c>
+      <c r="I3">
+        <v>3.3109999999999999</v>
+      </c>
+      <c r="J3">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="K3">
+        <v>3.5910000000000002</v>
+      </c>
+      <c r="L3">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="M3">
+        <v>1.494</v>
+      </c>
+      <c r="N3">
+        <v>0.997</v>
+      </c>
+      <c r="O3">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="P3">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>3.9049999999999998</v>
+      </c>
+      <c r="D4">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="E4">
+        <v>3.9060000000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="G4">
+        <v>2.0150000000000001</v>
+      </c>
+      <c r="H4">
+        <v>0.995</v>
+      </c>
+      <c r="I4">
+        <v>2.78</v>
+      </c>
+      <c r="J4">
+        <v>0.99</v>
+      </c>
+      <c r="K4">
+        <v>3.9049999999999998</v>
+      </c>
+      <c r="L4">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="M4">
+        <v>1.8859999999999999</v>
+      </c>
+      <c r="N4">
+        <v>0.996</v>
+      </c>
+      <c r="O4">
+        <v>1.4930000000000001</v>
+      </c>
+      <c r="P4">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>5.407</v>
+      </c>
+      <c r="D5">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="E5">
+        <v>5.407</v>
+      </c>
+      <c r="F5">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="G5">
+        <v>1.9019999999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.995</v>
+      </c>
+      <c r="I5">
+        <v>3.8149999999999999</v>
+      </c>
+      <c r="J5">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="K5">
+        <v>5.407</v>
+      </c>
+      <c r="L5">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="M5">
+        <v>2.2320000000000002</v>
+      </c>
+      <c r="N5">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="O5">
+        <v>1.524</v>
+      </c>
+      <c r="P5">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>3.6130249999999999E-14</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0.01</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.152</v>
+      </c>
+      <c r="H6">
+        <v>0.999</v>
+      </c>
+      <c r="I6">
+        <v>1.35</v>
+      </c>
+      <c r="J6">
+        <v>0.997</v>
+      </c>
+      <c r="K6" s="10">
+        <v>3.613E-14</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0.105</v>
+      </c>
+      <c r="N6">
+        <v>0.999</v>
+      </c>
+      <c r="O6">
+        <v>0.158</v>
+      </c>
+      <c r="P6">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>185.804</v>
+      </c>
+      <c r="D7">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="E7">
+        <v>185.804</v>
+      </c>
+      <c r="F7">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="G7">
+        <v>61.128999999999998</v>
+      </c>
+      <c r="H7">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="I7">
+        <v>167.83600000000001</v>
+      </c>
+      <c r="J7">
+        <v>0.86</v>
+      </c>
+      <c r="K7">
+        <v>185.804</v>
+      </c>
+      <c r="L7">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="M7">
+        <v>81.983999999999995</v>
+      </c>
+      <c r="N7">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="O7">
+        <v>59.24</v>
+      </c>
+      <c r="P7">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>43.131999999999998</v>
+      </c>
+      <c r="D8">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="E8">
+        <v>43.133000000000003</v>
+      </c>
+      <c r="F8">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="G8">
+        <v>44.802</v>
+      </c>
+      <c r="H8">
+        <v>0.99</v>
+      </c>
+      <c r="I8">
+        <v>70.512</v>
+      </c>
+      <c r="J8">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="K8">
+        <v>43.131999999999998</v>
+      </c>
+      <c r="L8">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="M8">
+        <v>36.259</v>
+      </c>
+      <c r="N8">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="O8">
+        <v>35.78</v>
+      </c>
+      <c r="P8">
+        <v>0.99399999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>43.579000000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="E9">
+        <v>43.579000000000001</v>
+      </c>
+      <c r="F9">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="G9">
+        <v>35.784999999999997</v>
+      </c>
+      <c r="H9">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="I9">
+        <v>42.865000000000002</v>
+      </c>
+      <c r="J9">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="K9">
+        <v>43.579000000000001</v>
+      </c>
+      <c r="L9">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="M9">
+        <v>31.704000000000001</v>
+      </c>
+      <c r="N9">
+        <v>0.995</v>
+      </c>
+      <c r="O9">
+        <v>31.161000000000001</v>
+      </c>
+      <c r="P9">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>8.8199999999999998E-13</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.01</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1.573</v>
+      </c>
+      <c r="H10">
+        <v>0.999</v>
+      </c>
+      <c r="I10">
+        <v>80.36</v>
+      </c>
+      <c r="J10">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="K10">
+        <v>8.8199999999999998E-13</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1.268</v>
+      </c>
+      <c r="N10">
+        <v>0.999</v>
+      </c>
+      <c r="O10">
+        <v>2.258</v>
+      </c>
+      <c r="P10">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>39.529000000000003</v>
+      </c>
+      <c r="D11">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="E11">
+        <v>39.53</v>
+      </c>
+      <c r="F11">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G11">
+        <v>15.17</v>
+      </c>
+      <c r="H11">
+        <v>0.996</v>
+      </c>
+      <c r="I11">
+        <v>71.864999999999995</v>
+      </c>
+      <c r="J11">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="K11">
+        <v>39.529000000000003</v>
+      </c>
+      <c r="L11">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="M11">
+        <v>17.044</v>
+      </c>
+      <c r="N11">
+        <v>0.995</v>
+      </c>
+      <c r="O11">
+        <v>11.081</v>
+      </c>
+      <c r="P11">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>39.889000000000003</v>
+      </c>
+      <c r="D12">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="E12">
+        <v>39.89</v>
+      </c>
+      <c r="F12">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="G12">
+        <v>9.8680000000000003</v>
+      </c>
+      <c r="H12">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="I12">
+        <v>58.781999999999996</v>
+      </c>
+      <c r="J12">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="K12">
+        <v>39.889000000000003</v>
+      </c>
+      <c r="L12">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="M12">
+        <v>25.611999999999998</v>
+      </c>
+      <c r="N12">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="O12">
+        <v>23.658000000000001</v>
+      </c>
+      <c r="P12">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>41.363</v>
+      </c>
+      <c r="D13">
+        <v>0.97</v>
+      </c>
+      <c r="E13">
+        <v>41.363999999999997</v>
+      </c>
+      <c r="F13">
+        <v>0.97</v>
+      </c>
+      <c r="G13">
+        <v>32.319000000000003</v>
+      </c>
+      <c r="H13">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="I13">
+        <v>52.198999999999998</v>
+      </c>
+      <c r="J13">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="K13">
+        <v>41.363</v>
+      </c>
+      <c r="L13">
+        <v>0.97</v>
+      </c>
+      <c r="M13">
+        <v>28.184000000000001</v>
+      </c>
+      <c r="N13">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="O13">
+        <v>27.463000000000001</v>
+      </c>
+      <c r="P13">
+        <v>0.98699999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>4.3860000000000002E-13</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0.01</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="H14">
+        <v>0.999</v>
+      </c>
+      <c r="I14">
+        <v>61.542000000000002</v>
+      </c>
+      <c r="J14">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="K14">
+        <v>4.3860000000000002E-13</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="P14">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>48.5</v>
+      </c>
+      <c r="D15">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="E15">
+        <v>48.499000000000002</v>
+      </c>
+      <c r="F15">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G15">
+        <v>17.852</v>
+      </c>
+      <c r="H15">
+        <v>0.997</v>
+      </c>
+      <c r="I15">
+        <v>66.218999999999994</v>
+      </c>
+      <c r="J15">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="K15">
+        <v>48.5</v>
+      </c>
+      <c r="L15">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="M15">
+        <v>21.077999999999999</v>
+      </c>
+      <c r="N15">
+        <v>0.995</v>
+      </c>
+      <c r="O15">
+        <v>14.228</v>
+      </c>
+      <c r="P15">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>6.4260000000000002</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>6.4279999999999999</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>9.3379999999999992</v>
+      </c>
+      <c r="H16">
+        <v>0.999</v>
+      </c>
+      <c r="I16">
+        <v>36.325000000000003</v>
+      </c>
+      <c r="J16">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="K16">
+        <v>6.4260000000000002</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>6.7270000000000003</v>
+      </c>
+      <c r="N16">
+        <v>0.999</v>
+      </c>
+      <c r="O16">
+        <v>7.3159999999999998</v>
+      </c>
+      <c r="P16">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>31.103999999999999</v>
+      </c>
+      <c r="D17">
+        <v>0.99</v>
+      </c>
+      <c r="E17">
+        <v>31.103000000000002</v>
+      </c>
+      <c r="F17">
+        <v>0.99</v>
+      </c>
+      <c r="G17">
+        <v>25.138999999999999</v>
+      </c>
+      <c r="H17">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="I17">
+        <v>46.482999999999997</v>
+      </c>
+      <c r="J17">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="K17">
+        <v>31.103999999999999</v>
+      </c>
+      <c r="L17">
+        <v>0.99</v>
+      </c>
+      <c r="M17">
+        <v>22.234000000000002</v>
+      </c>
+      <c r="N17">
+        <v>0.995</v>
+      </c>
+      <c r="O17">
+        <v>21.248999999999999</v>
+      </c>
+      <c r="P17">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="10">
+        <v>6.9544349999999999E-14</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0.01</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="H18">
+        <v>0.999</v>
+      </c>
+      <c r="I18">
+        <v>59.344000000000001</v>
+      </c>
+      <c r="J18">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="K18" s="10">
+        <v>6.9544999999999995E-14</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0.182</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>0.222</v>
+      </c>
+      <c r="P18">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J23" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L25">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="M25">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L26" s="7">
+        <v>31161</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L27">
+        <v>11.081</v>
+      </c>
+      <c r="M27">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L28" s="7">
+        <v>1519</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -985,34 +1982,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="9"/>
+      <c r="K1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="L1" s="9"/>
+      <c r="M1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4" t="s">
+      <c r="N1" s="9"/>
+      <c r="O1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="4"/>
+      <c r="P1" s="9"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1222,46 +2219,46 @@
         <v>19</v>
       </c>
       <c r="C6" s="2">
-        <v>3.1438429999999998E-13</v>
+        <v>3.1400000000000003E-13</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="2">
-        <v>1.0178E-2</v>
+        <v>0.01</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="2">
-        <v>5.6231000000000003E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="H6" s="2">
-        <v>0.99999400000000005</v>
+        <v>0.999</v>
       </c>
       <c r="I6" s="2">
-        <v>1.208405</v>
+        <v>1.208</v>
       </c>
       <c r="J6" s="2">
-        <v>0.99717199999999995</v>
+        <v>0.997</v>
       </c>
       <c r="K6" s="2">
-        <v>3.1438429999999998E-13</v>
+        <v>3.1429999999999998E-13</v>
       </c>
       <c r="L6" s="2">
         <v>1</v>
       </c>
       <c r="M6" s="2">
-        <v>3.1512999999999999E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="N6" s="2">
-        <v>0.99999800000000005</v>
+        <v>0.999</v>
       </c>
       <c r="O6" s="2">
-        <v>4.5643999999999997E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="P6" s="2">
-        <v>0.999996</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -1422,28 +2419,28 @@
         <v>19</v>
       </c>
       <c r="C10" s="2">
-        <v>1.331954E-13</v>
+        <v>1.3310000000000001E-13</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>1.0085999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10" s="2">
-        <v>0.46712100000000001</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="H10" s="2">
-        <v>0.99999899999999997</v>
+        <v>0.999</v>
       </c>
       <c r="I10" s="2">
-        <v>54.683965999999998</v>
+        <v>54.683999999999997</v>
       </c>
       <c r="J10" s="2">
-        <v>0.98627699999999996</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="K10" s="2">
         <v>1.331954E-13</v>
@@ -1452,16 +2449,16 @@
         <v>1</v>
       </c>
       <c r="M10" s="2">
-        <v>0.26831899999999997</v>
+        <v>0.26800000000000002</v>
       </c>
       <c r="N10" s="2">
         <v>1</v>
       </c>
       <c r="O10" s="2">
-        <v>0.42979200000000001</v>
+        <v>0.43</v>
       </c>
       <c r="P10" s="2">
-        <v>0.99999899999999997</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -1622,46 +2619,46 @@
         <v>19</v>
       </c>
       <c r="C14" s="2">
-        <v>3.7147349999999998E-13</v>
+        <v>3.7140000000000001E-13</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
       </c>
       <c r="E14" s="2">
-        <v>1.0175E-2</v>
+        <v>0.01</v>
       </c>
       <c r="F14" s="2">
         <v>1</v>
       </c>
       <c r="G14" s="2">
-        <v>0.318687</v>
+        <v>0.31900000000000001</v>
       </c>
       <c r="H14" s="2">
-        <v>0.99999800000000005</v>
+        <v>0.999</v>
       </c>
       <c r="I14" s="2">
-        <v>83.623318999999995</v>
+        <v>83.623000000000005</v>
       </c>
       <c r="J14" s="2">
-        <v>0.88862799999999997</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="K14" s="2">
-        <v>3.7147349999999998E-13</v>
+        <v>3.7140000000000001E-13</v>
       </c>
       <c r="L14" s="2">
         <v>1</v>
       </c>
       <c r="M14" s="2">
-        <v>0.14743600000000001</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="N14" s="2">
         <v>1</v>
       </c>
       <c r="O14" s="2">
-        <v>0.19586100000000001</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="P14" s="2">
-        <v>0.99999899999999997</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -1822,137 +2819,137 @@
         <v>19</v>
       </c>
       <c r="C18" s="2">
-        <v>3.1863629999999998E-13</v>
+        <v>3.1859999999999998E-13</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
       </c>
       <c r="E18" s="2">
-        <v>1.001E-2</v>
+        <v>0.01</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
       </c>
       <c r="G18" s="2">
-        <v>0.53312999999999999</v>
+        <v>0.53300000000000003</v>
       </c>
       <c r="H18" s="2">
-        <v>0.99999700000000002</v>
+        <v>0.999</v>
       </c>
       <c r="I18" s="2">
-        <v>74.224798000000007</v>
+        <v>74.224999999999994</v>
       </c>
       <c r="J18" s="2">
-        <v>0.94884599999999997</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="K18" s="2">
-        <v>3.1863629999999998E-13</v>
+        <v>3.1859999999999998E-13</v>
       </c>
       <c r="L18" s="2">
         <v>1</v>
       </c>
       <c r="M18" s="2">
-        <v>0.27301500000000001</v>
+        <v>0.27300000000000002</v>
       </c>
       <c r="N18" s="2">
-        <v>0.99999899999999997</v>
+        <v>0.999</v>
       </c>
       <c r="O18" s="2">
-        <v>0.34965400000000002</v>
+        <v>0.35</v>
       </c>
       <c r="P18" s="2">
-        <v>0.99999899999999997</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J22" s="6" t="s">
+      <c r="J22" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I23" s="7" t="s">
+      <c r="I23" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J23" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K23" s="7" t="s">
+      <c r="J23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L23" s="7" t="s">
+      <c r="L23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M23" s="7" t="s">
+      <c r="M23" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="J24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="K24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L24" s="8" t="s">
+      <c r="L24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M24" s="8" t="s">
+      <c r="M24" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="J25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="K25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25" s="7">
         <v>31259</v>
       </c>
-      <c r="M25" s="8" t="s">
+      <c r="M25" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="J26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="K26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L26" s="7">
         <v>15552</v>
       </c>
-      <c r="M26" s="8" t="s">
+      <c r="M26" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="I27" s="5" t="s">
+      <c r="I27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="J27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="K27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L27" s="9">
+      <c r="L27" s="7">
         <v>8905</v>
       </c>
-      <c r="M27" s="8" t="s">
+      <c r="M27" s="6" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1971,1003 +2968,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60578EB-98D6-4F88-B60F-5DF5FAA0FC36}">
-  <dimension ref="A1:P28"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4FF602-F8B4-4CAB-9238-8B147C5CF4E7}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23:M28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="4"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>3.5910000000000002</v>
-      </c>
-      <c r="D3">
-        <v>0.98399999999999999</v>
-      </c>
-      <c r="E3">
-        <v>3.5910000000000002</v>
-      </c>
-      <c r="F3">
-        <v>0.98399999999999999</v>
-      </c>
-      <c r="G3">
-        <v>1.349</v>
-      </c>
-      <c r="H3">
-        <v>0.998</v>
-      </c>
-      <c r="I3">
-        <v>3.3109999999999999</v>
-      </c>
-      <c r="J3">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="K3">
-        <v>3.5910000000000002</v>
-      </c>
-      <c r="L3">
-        <v>0.98399999999999999</v>
-      </c>
-      <c r="M3">
-        <v>1.494</v>
-      </c>
-      <c r="N3">
-        <v>0.997</v>
-      </c>
-      <c r="O3">
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="P3">
-        <v>0.999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>3.9049999999999998</v>
-      </c>
-      <c r="D4">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="E4">
-        <v>3.9060000000000001</v>
-      </c>
-      <c r="F4">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="G4">
-        <v>2.0150000000000001</v>
-      </c>
-      <c r="H4">
-        <v>0.995</v>
-      </c>
-      <c r="I4">
-        <v>2.78</v>
-      </c>
-      <c r="J4">
-        <v>0.99</v>
-      </c>
-      <c r="K4">
-        <v>3.9049999999999998</v>
-      </c>
-      <c r="L4">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="M4">
-        <v>1.8859999999999999</v>
-      </c>
-      <c r="N4">
-        <v>0.996</v>
-      </c>
-      <c r="O4">
-        <v>1.4930000000000001</v>
-      </c>
-      <c r="P4">
-        <v>0.997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>5.407</v>
-      </c>
-      <c r="D5">
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="E5">
-        <v>5.407</v>
-      </c>
-      <c r="F5">
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="G5">
-        <v>1.9019999999999999</v>
-      </c>
-      <c r="H5">
-        <v>0.995</v>
-      </c>
-      <c r="I5">
-        <v>3.8149999999999999</v>
-      </c>
-      <c r="J5">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="K5">
-        <v>5.407</v>
-      </c>
-      <c r="L5">
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="M5">
-        <v>2.2320000000000002</v>
-      </c>
-      <c r="N5">
-        <v>0.99399999999999999</v>
-      </c>
-      <c r="O5">
-        <v>1.524</v>
-      </c>
-      <c r="P5">
-        <v>0.997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>3.6130249999999999E-14</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0.01</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>0.152</v>
-      </c>
-      <c r="H6">
-        <v>0.999</v>
-      </c>
-      <c r="I6">
-        <v>1.35</v>
-      </c>
-      <c r="J6">
-        <v>0.997</v>
-      </c>
-      <c r="K6">
-        <v>3.6130249999999999E-14</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>0.105</v>
-      </c>
-      <c r="N6">
-        <v>0.999</v>
-      </c>
-      <c r="O6">
-        <v>0.158</v>
-      </c>
-      <c r="P6">
-        <v>0.999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>185.804</v>
-      </c>
-      <c r="D7">
-        <v>0.82899999999999996</v>
-      </c>
-      <c r="E7">
-        <v>185.804</v>
-      </c>
-      <c r="F7">
-        <v>0.82899999999999996</v>
-      </c>
-      <c r="G7">
-        <v>61.128999999999998</v>
-      </c>
-      <c r="H7">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="I7">
-        <v>167.83600000000001</v>
-      </c>
-      <c r="J7">
-        <v>0.86</v>
-      </c>
-      <c r="K7">
-        <v>185.804</v>
-      </c>
-      <c r="L7">
-        <v>0.82899999999999996</v>
-      </c>
-      <c r="M7">
-        <v>81.983999999999995</v>
-      </c>
-      <c r="N7">
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="O7">
-        <v>59.24</v>
-      </c>
-      <c r="P7">
-        <v>0.98299999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>43.131999999999998</v>
-      </c>
-      <c r="D8">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="E8">
-        <v>43.133000000000003</v>
-      </c>
-      <c r="F8">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="G8">
-        <v>44.802</v>
-      </c>
-      <c r="H8">
-        <v>0.99</v>
-      </c>
-      <c r="I8">
-        <v>70.512</v>
-      </c>
-      <c r="J8">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="K8">
-        <v>43.131999999999998</v>
-      </c>
-      <c r="L8">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="M8">
-        <v>36.259</v>
-      </c>
-      <c r="N8">
-        <v>0.99299999999999999</v>
-      </c>
-      <c r="O8">
-        <v>35.78</v>
-      </c>
-      <c r="P8">
-        <v>0.99399999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>43.579000000000001</v>
-      </c>
-      <c r="D9">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="E9">
-        <v>43.579000000000001</v>
-      </c>
-      <c r="F9">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="G9">
-        <v>35.784999999999997</v>
-      </c>
-      <c r="H9">
-        <v>0.99399999999999999</v>
-      </c>
-      <c r="I9">
-        <v>42.865000000000002</v>
-      </c>
-      <c r="J9">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="K9">
-        <v>43.579000000000001</v>
-      </c>
-      <c r="L9">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="M9">
-        <v>31.704000000000001</v>
-      </c>
-      <c r="N9">
-        <v>0.995</v>
-      </c>
-      <c r="O9">
-        <v>31.161000000000001</v>
-      </c>
-      <c r="P9">
-        <v>0.995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>8.8240699999999996E-13</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1.0071E-2</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1.573045</v>
-      </c>
-      <c r="H10">
-        <v>0.99998799999999999</v>
-      </c>
-      <c r="I10">
-        <v>80.360183000000006</v>
-      </c>
-      <c r="J10">
-        <v>0.96793200000000001</v>
-      </c>
-      <c r="K10">
-        <v>8.8240699999999996E-13</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>1.268221</v>
-      </c>
-      <c r="N10">
-        <v>0.99999199999999999</v>
-      </c>
-      <c r="O10">
-        <v>2.258041</v>
-      </c>
-      <c r="P10">
-        <v>0.99997499999999995</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>39.529000000000003</v>
-      </c>
-      <c r="D11">
-        <v>0.97199999999999998</v>
-      </c>
-      <c r="E11">
-        <v>39.53</v>
-      </c>
-      <c r="F11">
-        <v>0.97199999999999998</v>
-      </c>
-      <c r="G11">
-        <v>15.17</v>
-      </c>
-      <c r="H11">
-        <v>0.996</v>
-      </c>
-      <c r="I11">
-        <v>71.864999999999995</v>
-      </c>
-      <c r="J11">
-        <v>0.90900000000000003</v>
-      </c>
-      <c r="K11">
-        <v>39.529000000000003</v>
-      </c>
-      <c r="L11">
-        <v>0.97199999999999998</v>
-      </c>
-      <c r="M11">
-        <v>17.044</v>
-      </c>
-      <c r="N11">
-        <v>0.995</v>
-      </c>
-      <c r="O11">
-        <v>11.081</v>
-      </c>
-      <c r="P11">
-        <v>0.998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12">
-        <v>39.889000000000003</v>
-      </c>
-      <c r="D12">
-        <v>0.97199999999999998</v>
-      </c>
-      <c r="E12">
-        <v>39.89</v>
-      </c>
-      <c r="F12">
-        <v>0.97199999999999998</v>
-      </c>
-      <c r="G12">
-        <v>9.8680000000000003</v>
-      </c>
-      <c r="H12">
-        <v>0.98399999999999999</v>
-      </c>
-      <c r="I12">
-        <v>58.781999999999996</v>
-      </c>
-      <c r="J12">
-        <v>0.93899999999999995</v>
-      </c>
-      <c r="K12">
-        <v>39.889000000000003</v>
-      </c>
-      <c r="L12">
-        <v>0.97199999999999998</v>
-      </c>
-      <c r="M12">
-        <v>25.611999999999998</v>
-      </c>
-      <c r="N12">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="O12">
-        <v>23.658000000000001</v>
-      </c>
-      <c r="P12">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13">
-        <v>41.363</v>
-      </c>
-      <c r="D13">
-        <v>0.97</v>
-      </c>
-      <c r="E13">
-        <v>41.363999999999997</v>
-      </c>
-      <c r="F13">
-        <v>0.97</v>
-      </c>
-      <c r="G13">
-        <v>32.319000000000003</v>
-      </c>
-      <c r="H13">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="I13">
-        <v>52.198999999999998</v>
-      </c>
-      <c r="J13">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="K13">
-        <v>41.363</v>
-      </c>
-      <c r="L13">
-        <v>0.97</v>
-      </c>
-      <c r="M13">
-        <v>28.184000000000001</v>
-      </c>
-      <c r="N13">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="O13">
-        <v>27.463000000000001</v>
-      </c>
-      <c r="P13">
-        <v>0.98699999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14">
-        <v>4.3866690000000002E-13</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1.0213E-2</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>0.30281599999999997</v>
-      </c>
-      <c r="H14">
-        <v>0.99999800000000005</v>
-      </c>
-      <c r="I14">
-        <v>61.541727999999999</v>
-      </c>
-      <c r="J14">
-        <v>0.93302099999999999</v>
-      </c>
-      <c r="K14">
-        <v>4.3866690000000002E-13</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>0.162328</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14">
-        <v>0.339138</v>
-      </c>
-      <c r="P14">
-        <v>0.99999800000000005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>48.5</v>
-      </c>
-      <c r="D15">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="E15">
-        <v>48.499000000000002</v>
-      </c>
-      <c r="F15">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="G15">
-        <v>17.852</v>
-      </c>
-      <c r="H15">
-        <v>0.997</v>
-      </c>
-      <c r="I15">
-        <v>66.218999999999994</v>
-      </c>
-      <c r="J15">
-        <v>0.95399999999999996</v>
-      </c>
-      <c r="K15">
-        <v>48.5</v>
-      </c>
-      <c r="L15">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="M15">
-        <v>21.077999999999999</v>
-      </c>
-      <c r="N15">
-        <v>0.995</v>
-      </c>
-      <c r="O15">
-        <v>14.228</v>
-      </c>
-      <c r="P15">
-        <v>0.998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16">
-        <v>6.4260000000000002</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>6.4279999999999999</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>9.3379999999999992</v>
-      </c>
-      <c r="H16">
-        <v>0.999</v>
-      </c>
-      <c r="I16">
-        <v>36.325000000000003</v>
-      </c>
-      <c r="J16">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="K16">
-        <v>6.4260000000000002</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16">
-        <v>6.7270000000000003</v>
-      </c>
-      <c r="N16">
-        <v>0.999</v>
-      </c>
-      <c r="O16">
-        <v>7.3159999999999998</v>
-      </c>
-      <c r="P16">
-        <v>0.999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>31.103999999999999</v>
-      </c>
-      <c r="D17">
-        <v>0.99</v>
-      </c>
-      <c r="E17">
-        <v>31.103000000000002</v>
-      </c>
-      <c r="F17">
-        <v>0.99</v>
-      </c>
-      <c r="G17">
-        <v>25.138999999999999</v>
-      </c>
-      <c r="H17">
-        <v>0.99299999999999999</v>
-      </c>
-      <c r="I17">
-        <v>46.482999999999997</v>
-      </c>
-      <c r="J17">
-        <v>0.97699999999999998</v>
-      </c>
-      <c r="K17">
-        <v>31.103999999999999</v>
-      </c>
-      <c r="L17">
-        <v>0.99</v>
-      </c>
-      <c r="M17">
-        <v>22.234000000000002</v>
-      </c>
-      <c r="N17">
-        <v>0.995</v>
-      </c>
-      <c r="O17">
-        <v>21.248999999999999</v>
-      </c>
-      <c r="P17">
-        <v>0.995</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18">
-        <v>6.9544349999999999E-14</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>9.9150000000000002E-3</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>0.39926099999999998</v>
-      </c>
-      <c r="H18">
-        <v>0.99999800000000005</v>
-      </c>
-      <c r="I18">
-        <v>59.344006</v>
-      </c>
-      <c r="J18">
-        <v>0.96270599999999995</v>
-      </c>
-      <c r="K18">
-        <v>6.9544349999999999E-14</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
-        <v>0.18157999999999999</v>
-      </c>
-      <c r="N18">
-        <v>1</v>
-      </c>
-      <c r="O18">
-        <v>0.22176100000000001</v>
-      </c>
-      <c r="P18">
-        <v>0.99999899999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J23" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I24" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K24" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M24" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I25" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L25" s="9">
-        <v>1493</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I26" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L26" s="9">
-        <v>31161</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L27" s="9">
-        <v>10968</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I28" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L28" s="9">
-        <v>1519</v>
-      </c>
-      <c r="M28" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-  </mergeCells>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se arreglo el problema con las metricas de los modelos
</commit_message>
<xml_diff>
--- a/docs/metrics.xlsx
+++ b/docs/metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS TUF\Documents\repositorios\energy_consumption\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7106E1EC-0E0E-49F1-926F-0853FD0489FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AD19F2-163C-4C52-8942-9C836C2021B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clustering_results" sheetId="3" r:id="rId1"/>
@@ -508,13 +508,13 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60578EB-98D6-4F88-B60F-5DF5FAA0FC36}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,34 +973,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9" t="s">
+      <c r="J1" s="10"/>
+      <c r="K1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9" t="s">
+      <c r="L1" s="10"/>
+      <c r="M1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9" t="s">
+      <c r="N1" s="10"/>
+      <c r="O1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="9"/>
+      <c r="P1" s="10"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1233,7 +1233,7 @@
       <c r="J6">
         <v>0.997</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="8">
         <v>3.613E-14</v>
       </c>
       <c r="L6">
@@ -1809,7 +1809,7 @@
       <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="8">
         <v>6.9544349999999999E-14</v>
       </c>
       <c r="D18">
@@ -1833,7 +1833,7 @@
       <c r="J18">
         <v>0.96299999999999997</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="8">
         <v>6.9544999999999995E-14</v>
       </c>
       <c r="L18">
@@ -1853,11 +1853,11 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J23" s="8" t="s">
+      <c r="J23" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I24" s="5" t="s">
@@ -1932,7 +1932,7 @@
         <v>5</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>15</v>
@@ -1963,8 +1963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1982,34 +1982,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9" t="s">
+      <c r="J1" s="10"/>
+      <c r="K1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9" t="s">
+      <c r="L1" s="10"/>
+      <c r="M1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9" t="s">
+      <c r="N1" s="10"/>
+      <c r="O1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="9"/>
+      <c r="P1" s="10"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2862,11 +2862,11 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I23" s="5" t="s">

</xml_diff>